<commit_message>
updating terms in design pattern spreadsheet
</commit_message>
<xml_diff>
--- a/docs/MGPO Logical Definitions.xlsx
+++ b/docs/MGPO Logical Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-3936" yWindow="312" windowWidth="19140" windowHeight="8148"/>
+    <workbookView xWindow="-3936" yWindow="372" windowWidth="19140" windowHeight="8088"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,21 +78,21 @@
         </r>
         <r>
           <rPr>
-            <sz val="12"/>
+            <sz val="11"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">The need for classifying according to this characteristic is still under review.  
 Most phenotypes are reported in the literature or data sets are framed as abnormal levels of some glycan species.  Determining when such statements indicate a level-based phenotype (e.g. abnormal levels fucosylated glacans) vs. a composition-based phenotype (e.g. abnormal fucose content &gt; hyperfucosylation) is often ambiguous, and can require deeper analysis of the data and assumptions of the experimental design and interpretation (i.e. are authors concluding that there is a general increase in glycans that contain fucose, or are they concluding that specific species show increased fucose content?)
-Also, it is not clear if the underlying biological and genetic basis for these different phenotype categories is different enough to warrant distinguishing them in our model, nor is it clear if curators would be able to consistently distinguish which was appropriate  to annotate to.
+Also, it is not clear if the underlying biological and genetic basis for these different phenotype categories is different enough to warrant distinguishing them in our model, nor is it clear if curators would be able to consistently distinguish which was appropriate  to annotate to.  Finally, it is not clear if the utility for Phenosim use cases warrants this distinction.
 We are actively exploring these questions and considering curation practicalities to determine whether to model this distinction in our ontology.
 </t>
         </r>
         <r>
           <rPr>
             <b/>
-            <sz val="12"/>
+            <sz val="11"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -101,7 +101,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="12"/>
+            <sz val="11"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -155,13 +155,41 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This pattern requires that a specific residue type is used to be meaningful .  i.e. the expression below  that doesnt specify a specific residue type seems to say only that the glycan would hae an abnrommal length. 
+          <t xml:space="preserve">This pattern requires that a specific residue type is used to be meaningful .  i.e. the expression below  that doesnt specify a specific residue type seems to say only that the glycan would has an abnormal length. 
 'has part' some 
     ('altered number of'
      and ('inheres in' some glycan)
      and (towards some 'glycan residue')
      and ('has modifier' some abnormal))
-So, in our base design pattern, we use an 'X' to represent the specific residue that is abnormally represented (e.g. fucose, mannose, sialic acid, galactose, etc)</t>
+So, in our base design pattern the 'X'  represents the specific residue that is abnormally represented (e.g. fucose, mannose, sialic acid, galactose, etc)
+----
+Also note that the design pattern here is based on what may be an outdated approach, but I think it is necessary to specify the iintended meaning of these classes.  Recent documentation suggests that patterns such as this using a relational quality with </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>towards</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> shlould  be replaced by nested patterns such as:
+'has part' some 
+    ('altered number of'
+     and ('inheres in' some 
+         ('X glycan residue' and 
+        ('part of' some 'N-glycan chain')))
+     and ('has modifier' some abnormal))
+But this pattern is not precise enough - as it would be satisfied in a scenario where there is simply an increase in the total number of normal N-glycans in the cell . . . .i.e. it doesnt specify that the number is abnromal in the context of the glycan, as opposed to being abnormal in the context of the whose cell)</t>
         </r>
       </text>
     </comment>
@@ -285,6 +313,57 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Note that for occupancy, distinctions based on residues affected in the conjugated glycan likely isnt something we want to make classes for. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Brush:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Most of the secondary classifications for this primary characteristic will not yield impaortant classes, and can likely not be used to create new classes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Brush:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+GO describes binding as an activity / MF.  
+GO:0005488 binding has subclasses carbohydrate binding, and carbohydrate-derivative binding (follows ChEBI here).
+Not sure about the pattern of a qualitty inhering in a function that inehres in a molecular entity. 
+</t>
         </r>
       </text>
     </comment>
@@ -293,7 +372,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>has part' some 
     (amount
@@ -314,9 +393,6 @@
      and ('has modifier' some abnormal))</t>
   </si>
   <si>
-    <t>Modifying Dimension</t>
-  </si>
-  <si>
     <t>LEVELS</t>
   </si>
   <si>
@@ -330,9 +406,6 @@
   </si>
   <si>
     <t>An increase or decrease in the amount of a glycan present in the body, cell, or specific compartment  therein.</t>
-  </si>
-  <si>
-    <t>Abnormal Characteristic</t>
   </si>
   <si>
     <t>'abnormal levels free glycans'</t>
@@ -663,51 +736,12 @@
     </r>
   </si>
   <si>
-    <t>Abnormality
-Definition</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">has part' some 
-    ('altered number of'
-     and ('inheres in' some 
-         (glyco-conjugate 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">           and 'located in' some 'golgi complex'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>))
-     and (towards some 'glycan group')
-     and ('has modifier' some abnormal))</t>
-    </r>
-  </si>
-  <si>
     <t>'abnormal glycoprotein occupancy by
 terminally fucosylated glycans'</t>
   </si>
   <si>
     <t>'abnormal glycoprotein occupancy 
 by fucosylated glycans'</t>
-  </si>
-  <si>
-    <t>Base Eq Class Definition /
-Design Pattern</t>
   </si>
   <si>
     <t xml:space="preserve">   Glycan Characteristic Descriptions</t>
@@ -1072,19 +1106,264 @@
      and ('has modifier' some abnormal))</t>
     </r>
   </si>
+  <si>
+    <t>Primary Characteristic</t>
+  </si>
+  <si>
+    <t>Secondary/Modifying Dimension</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Base Equivalent Class Definition</t>
+  </si>
+  <si>
+    <t>BINDING</t>
+  </si>
+  <si>
+    <t>An increase or decrease in the binding efficacy of a glycan structure to a known binding partner.</t>
+  </si>
+  <si>
+    <t>has part' some 
+    (qualitative
+     and ('inheres in' some 
+        (binding and 
+           ('inheres in' some 
+             (glycan or glyco-conjugate))))
+     and ('has modifier' some abnormal))</t>
+  </si>
+  <si>
+    <r>
+      <t>has part' some 
+    (qualitative
+     and ('inheres in' some 
+        (binding and 
+           ('inheres in' some</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'N-glycan chain'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)))
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    (qualitative
+     and ('inheres in' some 
+        (binding and 
+           ('inheres in' some         
+            (glycan and 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">              ('bearer of' some 'detached from'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)))))
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    ('altered number of'
+     and ('inheres in' some 
+         (glyco-conjugate 
+             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and ('located in' some 'golgi complex'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>))
+     and (towards some 'glycan group')
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    (qualitative
+     and ('inheres in' some 
+        (binding and 
+           ('inheres in' some         
+            (glycan 
+              </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFCC00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  and  ('located in' some 'golgi complex')))))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     and ('has modifier' some abnormal))
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    (qualitative
+     and ('inheres in' some 
+        (binding and 
+           ('inheres in' some         
+            (glycan 
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      and  ('has part' some 'fucose residue'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)))))
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <t>'abnormal binding activity of N-glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of free-glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of glycans in the golgi'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of fucosylated glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of terminally fucosylated glycans'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    (qualitative
+     and ('inheres in' some 
+        (binding and 
+           ('inheres in' some         
+            (glycan 
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and  ('has part' some 'terminal fucose residue'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)))))
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1264,24 +1543,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color rgb="FFFFCC00"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1549,7 +1822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1575,10 +1848,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1604,16 +1877,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1634,86 +1907,89 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1723,9 +1999,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC00"/>
       <color rgb="FF969696"/>
       <color rgb="FFE0E0E0"/>
-      <color rgb="FFFFCC00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2025,21 +2301,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="27.109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="36.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="0.109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="39.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="41.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="41.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="38.88671875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="45.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="43.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="49.6640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="15.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2068,264 +2345,296 @@
       <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
-        <v>45</v>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42" t="s">
+        <v>40</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="26"/>
       <c r="F3" s="25"/>
       <c r="G3" s="26"/>
-      <c r="H3" s="54" t="s">
-        <v>3</v>
+      <c r="H3" s="40" t="s">
+        <v>57</v>
       </c>
       <c r="I3" s="26"/>
       <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>44</v>
+      <c r="B4" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="F4" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="53" t="s">
-        <v>55</v>
+      <c r="F4" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="31" t="s">
+      <c r="B5" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="47" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="44"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="28"/>
       <c r="F6" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>56</v>
+      <c r="B7" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>51</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="23" t="s">
         <v>19</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>21</v>
       </c>
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="106.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="33"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="28"/>
       <c r="F8" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
-      <c r="B9" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="34" t="s">
+      <c r="B9" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="43" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>24</v>
-      </c>
       <c r="I9" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="102.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="32"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="28"/>
       <c r="F10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="H10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
-      <c r="B11" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="31" t="s">
+      <c r="B11" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="47" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>35</v>
-      </c>
       <c r="I11" s="23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="33"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="29"/>
       <c r="F12" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+    <row r="14" spans="1:11" ht="130.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D15" s="4"/>
@@ -2401,19 +2710,22 @@
       <c r="E26" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
added v2 of mgpo to test new approach for first iteration of the module
</commit_message>
<xml_diff>
--- a/docs/MGPO Logical Definitions.xlsx
+++ b/docs/MGPO Logical Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-3936" yWindow="372" windowWidth="19140" windowHeight="8088"/>
+    <workbookView xWindow="-3936" yWindow="492" windowWidth="19140" windowHeight="7968"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -193,6 +194,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Brush:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Will likely want to frame this in terms of levels of glycans witih altered length - as this is how most are reported in the literature.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G11" authorId="0">
       <text>
         <r>
@@ -372,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>has part' some 
     (amount
@@ -1234,17 +1269,17 @@
         (binding and 
            ('inheres in' some         
             (glycan 
-              </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFCC00"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  and  ('located in' some 'golgi complex')))))</t>
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      and  ('has part' some 'fucose residue'</t>
     </r>
     <r>
       <rPr>
@@ -1254,20 +1289,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-     and ('has modifier' some abnormal))
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
+      <t>)))))
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <t>'abnormal binding activity of N-glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of free-glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of glycans in the golgi'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of fucosylated glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of terminally fucosylated glycans'</t>
   </si>
   <si>
     <r>
@@ -1287,7 +1326,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">      and  ('has part' some 'fucose residue'</t>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and  ('has part' some 'terminal fucose residue'</t>
     </r>
     <r>
       <rPr>
@@ -1302,19 +1351,61 @@
     </r>
   </si>
   <si>
-    <t>'abnormal binding activity of N-glycans'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of free-glycans'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of glycans in the golgi'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of fucosylated glycans'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of terminally fucosylated glycans'</t>
+    <t>Primary Characteristics</t>
+  </si>
+  <si>
+    <t>Secondary Modifiers</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Occupancy</t>
+  </si>
+  <si>
+    <t>Binding Activity</t>
+  </si>
+  <si>
+    <t>Glycan Class</t>
+  </si>
+  <si>
+    <t>Anatomical Location</t>
+  </si>
+  <si>
+    <t>Type of Residue Affected</t>
+  </si>
+  <si>
+    <t>Position of Residue Affected</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Attachment Status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+(free vs conjugated)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1324,27 +1415,17 @@
         (binding and 
            ('inheres in' some         
             (glycan 
-          </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and  ('has part' some 'terminal fucose residue'</t>
+              </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFCC00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  and  ('located in' some 'golgi complex')))))</t>
     </r>
     <r>
       <rPr>
@@ -1354,8 +1435,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)))))
+      <t xml:space="preserve">
      and ('has modifier' some abnormal))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
     </r>
   </si>
 </sst>
@@ -1363,7 +1454,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1556,8 +1647,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1594,8 +1698,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1818,11 +1934,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1864,9 +1995,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1946,50 +2074,92 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2301,14 +2471,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="3" customWidth="1"/>
     <col min="3" max="3" width="27.109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="36.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="0.109375" style="2" customWidth="1"/>
@@ -2321,103 +2491,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:11" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="40" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="38" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="46"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
@@ -2435,40 +2605,40 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="22" t="s">
+      <c r="E7" s="26"/>
+      <c r="F7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="22" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="106.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="15" t="s">
+      <c r="B8" s="57"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="42" t="s">
         <v>52</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -2487,40 +2657,40 @@
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="26"/>
+      <c r="F9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="22" t="s">
         <v>26</v>
       </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="102.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="16" t="s">
+      <c r="B10" s="65"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="15" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -2538,39 +2708,39 @@
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="26"/>
+      <c r="F11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="16" t="s">
+      <c r="B12" s="57"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="15" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -2588,52 +2758,52 @@
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="26"/>
+      <c r="F13" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="H13" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="J13" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="J13" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="130.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:11" ht="132.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="31" t="s">
+      <c r="B14" s="57"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="30" t="s">
         <v>63</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="J14" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2728,7 +2898,8 @@
     <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2746,12 +2917,76 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="16" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="50"/>
+      <c r="D4" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="16" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="50"/>
+      <c r="D6" s="46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="16" customFormat="1" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding files with exploratory approaches to classification
</commit_message>
<xml_diff>
--- a/docs/MGPO Logical Definitions.xlsx
+++ b/docs/MGPO Logical Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-3936" yWindow="492" windowWidth="19140" windowHeight="7968"/>
+    <workbookView xWindow="-3936" yWindow="552" windowWidth="19140" windowHeight="7908"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -463,36 +462,6 @@
     (amount
      and ('inheres in' some 
         (glycan
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">         and ('located in' some urine)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>))
-     and ('has modifier' some abnormal))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">has part' some 
-    (amount
-     and ('inheres in' some 
-        (glycan
          </t>
     </r>
     <r>
@@ -727,36 +696,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">         and ('bearer of' some 'detached from'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)))
-     and ('has modifier' some abnormal))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">has part' some 
-    (length
-     and ('inheres in' some 
-        (glycan
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">         and ('located in' some urine</t>
     </r>
     <r>
       <rPr>
@@ -1067,37 +1006,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> and ('bearer of' some 'detached from'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)))
-     and (towards some 'X glycan residue')
-     and ('has modifier' some abnormal))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">has part' some 
-    ('altered number of'
-     and ('inheres in' some
-        (glycan
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">         and ('located in' some urine</t>
     </r>
     <r>
       <rPr>
@@ -1233,20 +1141,22 @@
   <si>
     <r>
       <t xml:space="preserve">has part' some 
-    ('altered number of'
+    (qualitative
      and ('inheres in' some 
-         (glyco-conjugate 
-             </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and ('located in' some 'golgi complex'</t>
+        (binding and 
+           ('inheres in' some         
+            (glycan 
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      and  ('has part' some 'fucose residue'</t>
     </r>
     <r>
       <rPr>
@@ -1256,10 +1166,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>))
-     and (towards some 'glycan group')
+      <t>)))))
      and ('has modifier' some abnormal))</t>
     </r>
+  </si>
+  <si>
+    <t>'abnormal binding activity of N-glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of free-glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of glycans in the golgi'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of fucosylated glycans'</t>
+  </si>
+  <si>
+    <t>'abnormal binding activity of terminally fucosylated glycans'</t>
   </si>
   <si>
     <r>
@@ -1279,53 +1203,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">      and  ('has part' some 'fucose residue'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)))))
-     and ('has modifier' some abnormal))</t>
-    </r>
-  </si>
-  <si>
-    <t>'abnormal binding activity of N-glycans'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of free-glycans'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of glycans in the golgi'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of fucosylated glycans'</t>
-  </si>
-  <si>
-    <t>'abnormal binding activity of terminally fucosylated glycans'</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">has part' some 
-    (qualitative
-     and ('inheres in' some 
-        (binding and 
-           ('inheres in' some         
-            (glycan 
-          </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">      </t>
     </r>
     <r>
@@ -1405,6 +1282,128 @@
       </rPr>
       <t xml:space="preserve"> 
 (free vs conjugated)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    (amount
+     and ('inheres in' some 
+        (glycan
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">         and ('part of' some urine)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>))
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    ('altered number of'
+     and ('inheres in' some
+        (glycan
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">         and ('part of' some urine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)))
+     and (towards some 'X glycan residue')
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    (length
+     and ('inheres in' some 
+        (glycan
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">         and ('part of' some urine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)))
+     and ('has modifier' some abnormal))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has part' some 
+    ('altered number of'
+     and ('inheres in' some 
+         (glyco-conjugate 
+             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and ('part of' some 'golgi complex'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>))
+     and (towards some 'glycan group')
+     and ('has modifier' some abnormal))</t>
     </r>
   </si>
   <si>
@@ -1425,7 +1424,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  and  ('located in' some 'golgi complex')))))</t>
+      <t xml:space="preserve">  and  ('part of' some 'golgi complex')))))</t>
     </r>
     <r>
       <rPr>
@@ -2471,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2517,43 +2516,43 @@
     <row r="3" spans="1:11" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="40"/>
       <c r="C3" s="41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="25"/>
       <c r="F3" s="24"/>
       <c r="G3" s="25"/>
       <c r="H3" s="39" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>56</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>59</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="I4" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="J4" s="38" t="s">
         <v>48</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="38" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2568,13 +2567,13 @@
       </c>
       <c r="E5" s="26"/>
       <c r="F5" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>9</v>
@@ -2589,19 +2588,19 @@
       <c r="D6" s="62"/>
       <c r="E6" s="27"/>
       <c r="F6" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2609,10 +2608,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="21" t="s">
@@ -2622,13 +2621,13 @@
         <v>12</v>
       </c>
       <c r="H7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="J7" s="22" t="s">
         <v>18</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>19</v>
       </c>
       <c r="K7" s="10"/>
     </row>
@@ -2639,19 +2638,19 @@
       <c r="D8" s="61"/>
       <c r="E8" s="27"/>
       <c r="F8" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -2661,26 +2660,26 @@
         <v>5</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="67" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="26"/>
       <c r="F9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="H9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>22</v>
-      </c>
       <c r="I9" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -2691,19 +2690,19 @@
       <c r="D10" s="62"/>
       <c r="E10" s="27"/>
       <c r="F10" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="I10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2712,26 +2711,26 @@
         <v>6</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="H11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="22" t="s">
-        <v>33</v>
-      </c>
       <c r="I11" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2741,47 +2740,47 @@
       <c r="D12" s="61"/>
       <c r="E12" s="28"/>
       <c r="F12" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="I12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="56" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C13" s="58" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13" s="60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="21" t="s">
         <v>67</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="132.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2791,19 +2790,19 @@
       <c r="D14" s="61"/>
       <c r="E14" s="28"/>
       <c r="F14" s="30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>85</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2934,56 +2933,56 @@
     <row r="2" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="43"/>
       <c r="B2" s="44" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="44" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="16" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="51" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="51" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="46" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C4" s="50"/>
       <c r="D4" s="45" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="16" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="53" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="53" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="47" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C6" s="50"/>
       <c r="D6" s="46" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="16" customFormat="1" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="54" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="55" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>